<commit_message>
Added Authentication and integration
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/order.xlsx
+++ b/src/main/resources/excel/order.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>456</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>11231</t>
+  </si>
+  <si>
+    <t>od-856429</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>user101</t>
+  </si>
+  <si>
+    <t>2019-Sep-13</t>
   </si>
 </sst>
 </file>
@@ -382,6 +394,34 @@
     <row customFormat="1" r="2" spans="1:4" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="3" spans="1:4" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="4" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
UT and FT Test cases added for authentication and integration
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/order.xlsx
+++ b/src/main/resources/excel/order.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>456</t>
   </si>
@@ -380,29 +380,55 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="3" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="4" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="1" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -444,7 +470,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -478,20 +504,6 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added test cases for Services and Utils
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/order.xlsx
+++ b/src/main/resources/excel/order.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>456</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t xml:space="preserve">  102</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>G4234</t>
+  </si>
+  <si>
+    <t>2019-09-12T12:01:20.457Z</t>
   </si>
 </sst>
 </file>
@@ -380,7 +392,20 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s">
         <v>7</v>
@@ -428,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -439,72 +464,64 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>